<commit_message>
build ANOVA_df for TRA
</commit_message>
<xml_diff>
--- a/project_TRA/Holidays.xlsx
+++ b/project_TRA/Holidays.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PuSung\University\Sophomore\110-2 Academic\Satistics\Statistics_FinalProject\project_TRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEF6750-2206-4BAD-8D21-57C6D52D177D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC803B3-A7A9-4579-B6B3-727A842C65F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="10560" xr2:uid="{A6E7AF39-6FCD-4A1C-9E41-B61F33ABB7C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="11">
   <si>
     <t>日期</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>勞動</t>
-  </si>
-  <si>
-    <t>除夕</t>
   </si>
 </sst>
 </file>
@@ -413,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995D31EA-7060-4914-A266-2D0DAF7FC35E}">
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="F139" sqref="F139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,714 +522,714 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>38391</v>
+        <v>38745</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>38745</v>
+        <v>38868</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>38868</v>
+        <v>38996</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>38996</v>
+        <v>39000</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>39000</v>
+        <v>38776</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>38776</v>
+        <v>38717</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>38717</v>
+        <v>38812</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>38812</v>
+        <v>38836</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>38836</v>
+        <v>39130</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>38745</v>
+        <v>39249</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>39130</v>
+        <v>39347</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>39249</v>
+        <v>39365</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>39347</v>
+        <v>39141</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>39365</v>
+        <v>39081</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>39141</v>
+        <v>39177</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>39081</v>
+        <v>39203</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>39177</v>
+        <v>39484</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>39203</v>
+        <v>39606</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>39130</v>
+        <v>39704</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>39484</v>
+        <v>39731</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>39606</v>
+        <v>39506</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>39704</v>
+        <v>39448</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>39731</v>
+        <v>39542</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>39506</v>
+        <v>39569</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>39448</v>
+        <v>39837</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>39542</v>
+        <v>39961</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>39569</v>
+        <v>40089</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>39484</v>
+        <v>40096</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>39837</v>
+        <v>39872</v>
       </c>
       <c r="B38">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>39961</v>
+        <v>39814</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>40089</v>
+        <v>39907</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>40096</v>
+        <v>39934</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>39872</v>
+        <v>40222</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>39814</v>
+        <v>40345</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>39907</v>
+        <v>40443</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>39934</v>
+        <v>40460</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>39838</v>
+        <v>40236</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>40222</v>
+        <v>40179</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>40345</v>
+        <v>40271</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>40443</v>
+        <v>40299</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>40460</v>
+        <v>40576</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>40236</v>
+        <v>40698</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>40179</v>
+        <v>40796</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>40271</v>
+        <v>40824</v>
       </c>
       <c r="B53">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>40299</v>
+        <v>40600</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>40222</v>
+        <v>40544</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>40576</v>
+        <v>40635</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>40698</v>
+        <v>40663</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>40796</v>
+        <v>40929</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>40824</v>
+        <v>41083</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>40600</v>
+        <v>41181</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>40544</v>
+        <v>41192</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>40635</v>
+        <v>40234</v>
       </c>
       <c r="B62">
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>40663</v>
+        <v>40908</v>
       </c>
       <c r="B63">
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>40576</v>
+        <v>41003</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>40929</v>
+        <v>41030</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>41083</v>
+        <v>41314</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>41181</v>
+        <v>41437</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>41192</v>
+        <v>41536</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>40234</v>
+        <v>41557</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>40908</v>
+        <v>41333</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>41003</v>
+        <v>41272</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>41030</v>
+        <v>41368</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>40930</v>
+        <v>41395</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>41314</v>
+        <v>41669</v>
       </c>
       <c r="B74">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -1240,10 +1237,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>41437</v>
+        <v>41790</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
@@ -1251,10 +1248,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>41536</v>
+        <v>41888</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -1262,10 +1259,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>41557</v>
+        <v>41922</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
@@ -1273,10 +1270,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>41333</v>
+        <v>41698</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -1284,10 +1281,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>41272</v>
+        <v>41640</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -1295,10 +1292,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>41368</v>
+        <v>41733</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
@@ -1306,7 +1303,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>41395</v>
+        <v>41760</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -1317,904 +1314,706 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>41314</v>
+        <v>42053</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>41669</v>
+        <v>42174</v>
       </c>
       <c r="B83">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>41790</v>
+        <v>42273</v>
       </c>
       <c r="B84">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>41888</v>
+        <v>42286</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>41922</v>
+        <v>42062</v>
       </c>
       <c r="B86">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>41698</v>
+        <v>42005</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>41640</v>
+        <v>42097</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>41733</v>
+        <v>42125</v>
       </c>
       <c r="B89">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>41760</v>
+        <v>42406</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>41669</v>
+        <v>42530</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>42053</v>
+        <v>42628</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>42174</v>
+        <v>42652</v>
       </c>
       <c r="B93">
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>42273</v>
+        <v>42427</v>
       </c>
       <c r="B94">
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>42286</v>
+        <v>42370</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>42062</v>
+        <v>42462</v>
       </c>
       <c r="B96">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>42005</v>
+        <v>42490</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>42097</v>
+        <v>42762</v>
       </c>
       <c r="B98">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>42125</v>
+        <v>42882</v>
       </c>
       <c r="B99">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>42053</v>
+        <v>43012</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>42406</v>
+        <v>43015</v>
       </c>
       <c r="B101">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>42530</v>
+        <v>42791</v>
       </c>
       <c r="B102">
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>42628</v>
+        <v>42735</v>
       </c>
       <c r="B103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>42652</v>
+        <v>42826</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>42427</v>
+        <v>42854</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>42370</v>
+        <v>43146</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>42462</v>
+        <v>43267</v>
       </c>
       <c r="B107">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>42490</v>
+        <v>43365</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
-        <v>42407</v>
+        <v>43383</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>42762</v>
+        <v>43159</v>
       </c>
       <c r="B110">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>42882</v>
+        <v>43099</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
-        <v>43012</v>
+        <v>43194</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
-        <v>43015</v>
+        <v>43221</v>
       </c>
       <c r="B113">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <v>42791</v>
+        <v>43498</v>
       </c>
       <c r="B114">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>42735</v>
+        <v>43623</v>
       </c>
       <c r="B115">
         <v>3</v>
       </c>
       <c r="C115" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
-        <v>42826</v>
+        <v>43721</v>
       </c>
       <c r="B116">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
-        <v>42854</v>
+        <v>43748</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
-        <v>42762</v>
+        <v>43524</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
-        <v>43146</v>
+        <v>43463</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
-        <v>43267</v>
+        <v>43559</v>
       </c>
       <c r="B120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
-        <v>43365</v>
+        <v>43586</v>
       </c>
       <c r="B121">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>43383</v>
+        <v>43853</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C122" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
-        <v>43159</v>
+        <v>44007</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
-        <v>43099</v>
+        <v>44105</v>
       </c>
       <c r="B124">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
-        <v>43194</v>
+        <v>44113</v>
       </c>
       <c r="B125">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C125" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
-        <v>43221</v>
+        <v>43889</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
-        <v>43146</v>
+        <v>43831</v>
       </c>
       <c r="B127">
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
-        <v>43498</v>
+        <v>43923</v>
       </c>
       <c r="B128">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
-        <v>43623</v>
+        <v>43952</v>
       </c>
       <c r="B129">
         <v>3</v>
       </c>
       <c r="C129" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
-        <v>43721</v>
+        <v>44237</v>
       </c>
       <c r="B130">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
-        <v>43748</v>
+        <v>44359</v>
       </c>
       <c r="B131">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
-        <v>43524</v>
+        <v>44457</v>
       </c>
       <c r="B132">
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
-        <v>43463</v>
+        <v>44478</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
-        <v>43559</v>
+        <v>44254</v>
       </c>
       <c r="B134">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C134" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
-        <v>43586</v>
+        <v>44197</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
-        <v>43500</v>
+        <v>44288</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C136" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
-        <v>43853</v>
+        <v>44316</v>
       </c>
       <c r="B137">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C137" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
-        <v>44007</v>
+        <v>44590</v>
       </c>
       <c r="B138">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C138" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
-        <v>44105</v>
+        <v>44715</v>
       </c>
       <c r="B139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
-        <v>44113</v>
+        <v>44813</v>
       </c>
       <c r="B140">
         <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
-        <v>43889</v>
+        <v>44842</v>
       </c>
       <c r="B141">
         <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
-        <v>43831</v>
+        <v>44618</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
-        <v>43923</v>
+        <v>44561</v>
       </c>
       <c r="B143">
         <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
-        <v>43952</v>
+        <v>44653</v>
       </c>
       <c r="B144">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
-        <v>43854</v>
+        <v>44681</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="1">
-        <v>44237</v>
-      </c>
-      <c r="B146">
-        <v>7</v>
-      </c>
-      <c r="C146" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="1">
-        <v>44359</v>
-      </c>
-      <c r="B147">
-        <v>3</v>
-      </c>
-      <c r="C147" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="1">
-        <v>44457</v>
-      </c>
-      <c r="B148">
-        <v>4</v>
-      </c>
-      <c r="C148" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="1">
-        <v>44478</v>
-      </c>
-      <c r="B149">
-        <v>3</v>
-      </c>
-      <c r="C149" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="1">
-        <v>44254</v>
-      </c>
-      <c r="B150">
-        <v>3</v>
-      </c>
-      <c r="C150" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="1">
-        <v>44197</v>
-      </c>
-      <c r="B151">
-        <v>3</v>
-      </c>
-      <c r="C151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="1">
-        <v>44288</v>
-      </c>
-      <c r="B152">
-        <v>4</v>
-      </c>
-      <c r="C152" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="1">
-        <v>44316</v>
-      </c>
-      <c r="B153">
-        <v>3</v>
-      </c>
-      <c r="C153" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="1">
-        <v>44238</v>
-      </c>
-      <c r="B154">
-        <v>1</v>
-      </c>
-      <c r="C154" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="1">
-        <v>44590</v>
-      </c>
-      <c r="B155">
-        <v>9</v>
-      </c>
-      <c r="C155" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="1">
-        <v>44715</v>
-      </c>
-      <c r="B156">
-        <v>3</v>
-      </c>
-      <c r="C156" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="1">
-        <v>44813</v>
-      </c>
-      <c r="B157">
-        <v>3</v>
-      </c>
-      <c r="C157" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="1">
-        <v>44842</v>
-      </c>
-      <c r="B158">
-        <v>3</v>
-      </c>
-      <c r="C158" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" s="1">
-        <v>44618</v>
-      </c>
-      <c r="B159">
-        <v>3</v>
-      </c>
-      <c r="C159" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="1">
-        <v>44561</v>
-      </c>
-      <c r="B160">
-        <v>3</v>
-      </c>
-      <c r="C160" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="1">
-        <v>44653</v>
-      </c>
-      <c r="B161">
-        <v>4</v>
-      </c>
-      <c r="C161" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="1">
-        <v>44681</v>
-      </c>
-      <c r="B162">
-        <v>3</v>
-      </c>
-      <c r="C162" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="1">
-        <v>44592</v>
-      </c>
-      <c r="B163">
-        <v>1</v>
-      </c>
-      <c r="C163" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>